<commit_message>
globaladmin added as default in zone-user tables.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/xlsx/zone_user.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/xlsx/zone_user.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -32,15 +32,28 @@
   </si>
   <si>
     <t xml:space="preserve">is_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globaladmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -122,7 +135,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,6 +146,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -152,13 +173,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576 1:1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.6"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -172,6 +197,34 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>